<commit_message>
patch novendra, quiz sebelum perbaikan view
</commit_message>
<xml_diff>
--- a/public/be_assets/quiz/tempImportQuiz.xlsx
+++ b/public/be_assets/quiz/tempImportQuiz.xlsx
@@ -113,10 +113,10 @@
     <t>skip</t>
   </si>
   <si>
-    <t>be_assets\quiz\quiz_0467c42c-25eb-4b01-b073-509a2ceca9ca.png</t>
-  </si>
-  <si>
-    <t>be_assets\quiz\quiz_3db04a8b-ae4b-49a3-9b6c-f492804111db.png</t>
+    <t>be_assets\quiz\quiz_0f13a20c-16f0-4fbf-a33f-c6cecf985e19.png</t>
+  </si>
+  <si>
+    <t>be_assets\quiz\quiz_9fe95eef-eb1c-4350-a67f-d437a7203f5a.png</t>
   </si>
 </sst>
 </file>
@@ -536,8 +536,8 @@
   </sheetPr>
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1" topLeftCell="A4">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1" topLeftCell="A8">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>